<commit_message>
added details for copula
</commit_message>
<xml_diff>
--- a/projects/CopulaUnitTest.xlsx
+++ b/projects/CopulaUnitTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hongm\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5668D275-0523-4F08-8D79-24B51A863785}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203C79D4-86AA-48DE-8298-5FB23147524A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="6975" xr2:uid="{B2B9CE8E-42C4-48A3-8D4D-C26F0FF46720}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="6975" firstSheet="2" activeTab="4" xr2:uid="{B2B9CE8E-42C4-48A3-8D4D-C26F0FF46720}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelServiceTest" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Simulation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9369105-64ED-43B5-B70B-9AA4C6F9BD94}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -596,305 +596,385 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>_xll.ModelService_Version()</f>
+        <f ca="1">_xll.ModelService_Version()</f>
         <v>Copula Service: Version 1.0.0, Build on 2020-02-02</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="str">
-        <f t="array" ref="B3:D29">_xll.ModelService_DisplayFunctions()</f>
+        <f t="array" aca="1" ref="B3:D29" ca="1">_xll.ModelService_DisplayFunctions()</f>
         <v>ModelService_Version</v>
       </c>
       <c r="C3" t="str">
+        <f ca="1"/>
         <v>Version Information</v>
       </c>
       <c r="D3" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
+        <f ca="1"/>
         <v>CopulaService_GaussianCalibration</v>
       </c>
       <c r="C4" t="str">
-        <v>Calibrate Calibration Copula</v>
+        <f ca="1"/>
+        <v>Calibrate Gaussian Copula</v>
       </c>
       <c r="D4" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="str">
+        <f ca="1"/>
         <v>CopulaService_StudentCalibration</v>
       </c>
       <c r="C5" t="str">
+        <f ca="1"/>
         <v>Calibrate Student Copula</v>
       </c>
       <c r="D5" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
+        <f ca="1"/>
         <v>CopulaService_ArchimedeanCalibration</v>
       </c>
       <c r="C6" t="str">
+        <f ca="1"/>
         <v>Calibrate Archimedean Copula</v>
       </c>
       <c r="D6" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
+        <f ca="1"/>
         <v>CopulaService_GaussianSimulation</v>
       </c>
       <c r="C7" t="str">
-        <v>Simulate Calibration Copula</v>
+        <f ca="1"/>
+        <v>Simulate Gaussian Copula</v>
       </c>
       <c r="D7" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
+        <f ca="1"/>
         <v>CopulaService_StudentSimulation</v>
       </c>
       <c r="C8" t="str">
+        <f ca="1"/>
         <v>Simulate Student Copula</v>
       </c>
       <c r="D8" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
+        <f ca="1"/>
         <v>CopulaService_ArchimedeanSimulation</v>
       </c>
       <c r="C9" t="str">
+        <f ca="1"/>
         <v>Simulate Archimedean Copula</v>
       </c>
       <c r="D9" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
+        <f ca="1"/>
         <v>SmoothingService_KernelSmoothing</v>
       </c>
       <c r="C10" t="str">
+        <f ca="1"/>
         <v>Smooth Discrete Data using Kernel Functions</v>
       </c>
       <c r="D10" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C11" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D11" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C12" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D12" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C13" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D13" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C14" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D14" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C15" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D15" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C16" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D16" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C17" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D17" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C18" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D18" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C19" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D19" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C20" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D20" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C21" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D21" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C22" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D22" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C23" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D23" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C24" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D24" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C25" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D25" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C26" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D26" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C27" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D27" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C28" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D28" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="C29" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
       <c r="D29" t="e">
+        <f ca="1"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -909,7 +989,7 @@
   <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1002,7 +1082,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f ca="1">RAND()</f>
+        <f t="shared" ref="A11:A42" ca="1" si="0">RAND()</f>
         <v>0.15779145137124906</v>
       </c>
       <c r="C11">
@@ -1021,13 +1101,13 @@
         <v>1.7122267577881489E-3</v>
       </c>
       <c r="H11">
-        <f ca="1">VLOOKUP(G11,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ref="H11:H42" ca="1" si="1">VLOOKUP(G11,$C$11:$D$210,2,FALSE)</f>
         <v>5.5419704211292053E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.17218715405005902</v>
       </c>
       <c r="C12">
@@ -1046,13 +1126,13 @@
         <v>2.9796771519022824E-3</v>
       </c>
       <c r="H12">
-        <f ca="1">VLOOKUP(G12,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>5.6041279426788763E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.70536421020951268</v>
       </c>
       <c r="C13">
@@ -1071,13 +1151,13 @@
         <v>1.078728996835554E-2</v>
       </c>
       <c r="H13">
-        <f ca="1">VLOOKUP(G13,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>5.9970537906788017E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.28052096720332098</v>
       </c>
       <c r="C14">
@@ -1096,13 +1176,13 @@
         <v>1.0898239752113237E-2</v>
       </c>
       <c r="H14">
-        <f ca="1">VLOOKUP(G14,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>6.0027616146287752E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.96899087623978364</v>
       </c>
       <c r="C15">
@@ -1121,13 +1201,13 @@
         <v>1.7337165596859161E-2</v>
       </c>
       <c r="H15">
-        <f ca="1">VLOOKUP(G15,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>6.3400345298534055E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.90949156806361353</v>
       </c>
       <c r="C16">
@@ -1146,13 +1226,13 @@
         <v>2.4108168228572757E-2</v>
       </c>
       <c r="H16">
-        <f ca="1">VLOOKUP(G16,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>6.7073406159523549E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.90509923036776352</v>
       </c>
       <c r="C17">
@@ -1171,13 +1251,13 @@
         <v>2.7217525751247695E-2</v>
       </c>
       <c r="H17">
-        <f ca="1">VLOOKUP(G17,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>6.8803534479833922E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.36404804489053422</v>
       </c>
       <c r="C18">
@@ -1196,13 +1276,13 @@
         <v>3.2521870340801673E-2</v>
       </c>
       <c r="H18">
-        <f ca="1">VLOOKUP(G18,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>7.1818264741800975E-2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.5415391865705288</v>
       </c>
       <c r="C19">
@@ -1221,13 +1301,13 @@
         <v>4.0814367675169105E-2</v>
       </c>
       <c r="H19">
-        <f ca="1">VLOOKUP(G19,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>7.6689733675049804E-2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.6601836508485609</v>
       </c>
       <c r="C20">
@@ -1246,13 +1326,13 @@
         <v>4.7905004736181089E-2</v>
       </c>
       <c r="H20">
-        <f ca="1">VLOOKUP(G20,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>8.1007400250956707E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.62188519028793798</v>
       </c>
       <c r="C21">
@@ -1271,13 +1351,13 @@
         <v>5.074436438629315E-2</v>
       </c>
       <c r="H21">
-        <f ca="1">VLOOKUP(G21,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>8.2775343072582649E-2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.9931097264999057</v>
       </c>
       <c r="C22">
@@ -1296,13 +1376,13 @@
         <v>6.4992667140739258E-2</v>
       </c>
       <c r="H22">
-        <f ca="1">VLOOKUP(G22,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9.1979451341149029E-2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.23743474559263933</v>
       </c>
       <c r="C23">
@@ -1321,13 +1401,13 @@
         <v>6.6968298801553194E-2</v>
       </c>
       <c r="H23">
-        <f ca="1">VLOOKUP(G23,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9.3298679573157559E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.88889517457113931</v>
       </c>
       <c r="C24">
@@ -1346,13 +1426,13 @@
         <v>7.5311310574320056E-2</v>
       </c>
       <c r="H24">
-        <f ca="1">VLOOKUP(G24,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9.8983698191252828E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.71990193612817688</v>
       </c>
       <c r="C25">
@@ -1371,13 +1451,13 @@
         <v>8.1998452374188679E-2</v>
       </c>
       <c r="H25">
-        <f ca="1">VLOOKUP(G25,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.10367061511698003</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.15225811821584279</v>
       </c>
       <c r="C26">
@@ -1396,13 +1476,13 @@
         <v>8.991668778013151E-2</v>
       </c>
       <c r="H26">
-        <f ca="1">VLOOKUP(G26,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.10936711554328793</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.25921650782268923</v>
       </c>
       <c r="C27">
@@ -1421,13 +1501,13 @@
         <v>9.4612651860831454E-2</v>
       </c>
       <c r="H27">
-        <f ca="1">VLOOKUP(G27,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1128186489942011</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.90429427604463253</v>
       </c>
       <c r="C28">
@@ -1446,13 +1526,13 @@
         <v>9.7837835960232544E-2</v>
       </c>
       <c r="H28">
-        <f ca="1">VLOOKUP(G28,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.11522031323604791</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.7905004736181089E-2</v>
       </c>
       <c r="C29">
@@ -1471,13 +1551,13 @@
         <v>0.11942318801088558</v>
       </c>
       <c r="H29">
-        <f ca="1">VLOOKUP(G29,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1319135548342501</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.64812661935620586</v>
       </c>
       <c r="C30">
@@ -1496,13 +1576,13 @@
         <v>0.12186110338312595</v>
       </c>
       <c r="H30">
-        <f ca="1">VLOOKUP(G30,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.13386398005226402</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.31897613902624289</v>
       </c>
       <c r="C31">
@@ -1521,13 +1601,13 @@
         <v>0.12204445810335407</v>
       </c>
       <c r="H31">
-        <f ca="1">VLOOKUP(G31,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.13401116995121809</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.42934979603996137</v>
       </c>
       <c r="C32">
@@ -1546,13 +1626,13 @@
         <v>0.12274987953796856</v>
       </c>
       <c r="H32">
-        <f ca="1">VLOOKUP(G32,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1345781148034122</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.37356190579633497</v>
       </c>
       <c r="C33">
@@ -1571,13 +1651,13 @@
         <v>0.12367011636589187</v>
       </c>
       <c r="H33">
-        <f ca="1">VLOOKUP(G33,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1353192764490089</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.20600152094459301</v>
       </c>
       <c r="C34">
@@ -1596,13 +1676,13 @@
         <v>0.13500690479601085</v>
       </c>
       <c r="H34">
-        <f ca="1">VLOOKUP(G34,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.14459273290049959</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.86500894223247471</v>
       </c>
       <c r="C35">
@@ -1621,13 +1701,13 @@
         <v>0.13775098820824261</v>
       </c>
       <c r="H35">
-        <f ca="1">VLOOKUP(G35,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.1468755148661274</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.49218259729089975</v>
       </c>
       <c r="C36">
@@ -1646,13 +1726,13 @@
         <v>0.15225811821584279</v>
       </c>
       <c r="H36">
-        <f ca="1">VLOOKUP(G36,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.15917641121874537</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.82249681530953922</v>
       </c>
       <c r="C37">
@@ -1671,13 +1751,13 @@
         <v>0.15262259680293022</v>
       </c>
       <c r="H37">
-        <f ca="1">VLOOKUP(G37,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.15949024992361807</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.90724442186076137</v>
       </c>
       <c r="C38">
@@ -1696,13 +1776,13 @@
         <v>0.15296470412084306</v>
       </c>
       <c r="H38">
-        <f ca="1">VLOOKUP(G38,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.15978503113955772</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.33360256140495403</v>
       </c>
       <c r="C39">
@@ -1721,13 +1801,13 @@
         <v>0.15779145137124906</v>
       </c>
       <c r="H39">
-        <f ca="1">VLOOKUP(G39,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.16396510404838849</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.16728228026129344</v>
       </c>
       <c r="C40">
@@ -1746,13 +1826,13 @@
         <v>0.16728228026129344</v>
       </c>
       <c r="H40">
-        <f ca="1">VLOOKUP(G40,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.17229325965341377</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.64104700133711212</v>
       </c>
       <c r="C41">
@@ -1771,13 +1851,13 @@
         <v>0.16779134635167114</v>
       </c>
       <c r="H41">
-        <f ca="1">VLOOKUP(G41,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.17274386087844698</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.71942704459791362</v>
       </c>
       <c r="C42">
@@ -1796,13 +1876,13 @@
         <v>0.17218715405005902</v>
       </c>
       <c r="H42">
-        <f ca="1">VLOOKUP(G42,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.17665059971930738</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
-        <f ca="1">RAND()</f>
+        <f t="shared" ref="A43:A74" ca="1" si="2">RAND()</f>
         <v>0.88976342202478631</v>
       </c>
       <c r="C43">
@@ -1821,13 +1901,13 @@
         <v>0.17334968426002795</v>
       </c>
       <c r="H43">
-        <f ca="1">VLOOKUP(G43,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ref="H43:H74" ca="1" si="3">VLOOKUP(G43,$C$11:$D$210,2,FALSE)</f>
         <v>0.17768842206733798</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.48754617572371206</v>
       </c>
       <c r="C44">
@@ -1846,13 +1926,13 @@
         <v>0.17510853168654139</v>
       </c>
       <c r="H44">
-        <f ca="1">VLOOKUP(G44,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.17926218518308334</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.95685108731212942</v>
       </c>
       <c r="C45">
@@ -1871,13 +1951,13 @@
         <v>0.1753419963207854</v>
       </c>
       <c r="H45">
-        <f ca="1">VLOOKUP(G45,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.1794714038126434</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.81446791254319073</v>
       </c>
       <c r="C46">
@@ -1896,13 +1976,13 @@
         <v>0.17588953604697677</v>
       </c>
       <c r="H46">
-        <f ca="1">VLOOKUP(G46,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.17996237288590977</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.67048525519173185</v>
       </c>
       <c r="C47">
@@ -1921,13 +2001,13 @@
         <v>0.17888722108740762</v>
       </c>
       <c r="H47">
-        <f ca="1">VLOOKUP(G47,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.18265763079176178</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.9258348840460412</v>
       </c>
       <c r="C48">
@@ -1946,13 +2026,13 @@
         <v>0.18218204092391144</v>
       </c>
       <c r="H48">
-        <f ca="1">VLOOKUP(G48,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.18563360785780098</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.80401721435042617</v>
       </c>
       <c r="C49">
@@ -1971,13 +2051,13 @@
         <v>0.18384129893805279</v>
       </c>
       <c r="H49">
-        <f ca="1">VLOOKUP(G49,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.18713755581911282</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>2.4108168228572757E-2</v>
       </c>
       <c r="C50">
@@ -1996,13 +2076,13 @@
         <v>0.19206669044047031</v>
       </c>
       <c r="H50">
-        <f ca="1">VLOOKUP(G50,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.19464240836409943</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.95616580382950833</v>
       </c>
       <c r="C51">
@@ -2021,13 +2101,13 @@
         <v>0.19281679903418802</v>
       </c>
       <c r="H51">
-        <f ca="1">VLOOKUP(G51,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.1953307208888152</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.13775098820824261</v>
       </c>
       <c r="C52">
@@ -2046,13 +2126,13 @@
         <v>0.20600152094459301</v>
       </c>
       <c r="H52">
-        <f ca="1">VLOOKUP(G52,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.20752645926447694</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.61311987827802683</v>
       </c>
       <c r="C53">
@@ -2071,13 +2151,13 @@
         <v>0.20732584521069475</v>
       </c>
       <c r="H53">
-        <f ca="1">VLOOKUP(G53,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.20876083990697397</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.99121748500782902</v>
       </c>
       <c r="C54">
@@ -2096,13 +2176,13 @@
         <v>0.21195144677754441</v>
       </c>
       <c r="H54">
-        <f ca="1">VLOOKUP(G54,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.2130847747090083</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.62498956591875154</v>
       </c>
       <c r="C55">
@@ -2121,13 +2201,13 @@
         <v>0.23036853383573574</v>
       </c>
       <c r="H55">
-        <f ca="1">VLOOKUP(G55,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.23046424921338735</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>9.4612651860831454E-2</v>
       </c>
       <c r="C56">
@@ -2146,13 +2226,13 @@
         <v>0.23718011017572782</v>
       </c>
       <c r="H56">
-        <f ca="1">VLOOKUP(G56,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.23694728349307928</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.16779134635167114</v>
       </c>
       <c r="C57">
@@ -2171,13 +2251,13 @@
         <v>0.23743474559263933</v>
       </c>
       <c r="H57">
-        <f ca="1">VLOOKUP(G57,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.23719009368757968</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.33284561754969866</v>
       </c>
       <c r="C58">
@@ -2196,13 +2276,13 @@
         <v>0.2458915566478147</v>
       </c>
       <c r="H58">
-        <f ca="1">VLOOKUP(G58,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.24527135992771712</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.43415476418794674</v>
       </c>
       <c r="C59">
@@ -2221,13 +2301,13 @@
         <v>0.24769012162883808</v>
       </c>
       <c r="H59">
-        <f ca="1">VLOOKUP(G59,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.24699382222576016</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.69739651627477239</v>
       </c>
       <c r="C60">
@@ -2246,13 +2326,13 @@
         <v>0.25807125956454957</v>
       </c>
       <c r="H60">
-        <f ca="1">VLOOKUP(G60,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.25695729765645819</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.26878778962594108</v>
       </c>
       <c r="C61">
@@ -2271,13 +2351,13 @@
         <v>0.25921650782268923</v>
       </c>
       <c r="H61">
-        <f ca="1">VLOOKUP(G61,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.25805825833139895</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.24769012162883808</v>
       </c>
       <c r="C62">
@@ -2296,13 +2376,13 @@
         <v>0.26000782796753508</v>
       </c>
       <c r="H62">
-        <f ca="1">VLOOKUP(G62,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.25881915585084547</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.69325810791722031</v>
       </c>
       <c r="C63">
@@ -2321,13 +2401,13 @@
         <v>0.26878778962594108</v>
       </c>
       <c r="H63">
-        <f ca="1">VLOOKUP(G63,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.26727002534925182</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.32068602217968323</v>
       </c>
       <c r="C64">
@@ -2346,13 +2426,13 @@
         <v>0.27180867579582779</v>
       </c>
       <c r="H64">
-        <f ca="1">VLOOKUP(G64,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.27018026455311145</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.33227159518526728</v>
       </c>
       <c r="C65">
@@ -2371,13 +2451,13 @@
         <v>0.27228545150351047</v>
       </c>
       <c r="H65">
-        <f ca="1">VLOOKUP(G65,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.27063966696179687</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.78095119462370055</v>
       </c>
       <c r="C66">
@@ -2396,13 +2476,13 @@
         <v>0.27377111072492943</v>
       </c>
       <c r="H66">
-        <f ca="1">VLOOKUP(G66,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.27207144143007278</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.58677414175122655</v>
       </c>
       <c r="C67">
@@ -2421,13 +2501,13 @@
         <v>0.28052096720332098</v>
       </c>
       <c r="H67">
-        <f ca="1">VLOOKUP(G67,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.27857772562244887</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.76583932087094808</v>
       </c>
       <c r="C68">
@@ -2446,13 +2526,13 @@
         <v>0.28786506553522451</v>
       </c>
       <c r="H68">
-        <f ca="1">VLOOKUP(G68,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.2856577629156738</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.61649041736527788</v>
       </c>
       <c r="C69">
@@ -2471,13 +2551,13 @@
         <v>0.29120229052045066</v>
       </c>
       <c r="H69">
-        <f ca="1">VLOOKUP(G69,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.28887447882505385</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.92766017343413176</v>
       </c>
       <c r="C70">
@@ -2496,13 +2576,13 @@
         <v>0.29376542857156063</v>
       </c>
       <c r="H70">
-        <f ca="1">VLOOKUP(G70,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.29134455867951775</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.25807125956454957</v>
       </c>
       <c r="C71">
@@ -2521,13 +2601,13 @@
         <v>0.29668229901792387</v>
       </c>
       <c r="H71">
-        <f ca="1">VLOOKUP(G71,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.29415464225164389</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.57117856170137415</v>
       </c>
       <c r="C72">
@@ -2546,13 +2626,13 @@
         <v>0.30165133066451744</v>
       </c>
       <c r="H72">
-        <f ca="1">VLOOKUP(G72,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.29893959928263764</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.66416482932904097</v>
       </c>
       <c r="C73">
@@ -2571,13 +2651,13 @@
         <v>0.31631483575615282</v>
       </c>
       <c r="H73">
-        <f ca="1">VLOOKUP(G73,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.31303605149163027</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0.31631483575615282</v>
       </c>
       <c r="C74">
@@ -2596,13 +2676,13 @@
         <v>0.31897613902624289</v>
       </c>
       <c r="H74">
-        <f ca="1">VLOOKUP(G74,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0.31558988198834953</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75">
-        <f ca="1">RAND()</f>
+        <f t="shared" ref="A75:A106" ca="1" si="4">RAND()</f>
         <v>1.0898239752113237E-2</v>
       </c>
       <c r="C75">
@@ -2621,13 +2701,13 @@
         <v>0.32017316355401948</v>
       </c>
       <c r="H75">
-        <f ca="1">VLOOKUP(G75,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ref="H75:H106" ca="1" si="5">VLOOKUP(G75,$C$11:$D$210,2,FALSE)</f>
         <v>0.31673788774769823</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.40825151308399987</v>
       </c>
       <c r="C76">
@@ -2646,13 +2726,13 @@
         <v>0.32043577670379675</v>
       </c>
       <c r="H76">
-        <f ca="1">VLOOKUP(G76,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.31698969983548048</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.87600668101402845</v>
       </c>
       <c r="C77">
@@ -2671,13 +2751,13 @@
         <v>0.32045032100106585</v>
       </c>
       <c r="H77">
-        <f ca="1">VLOOKUP(G77,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.31700364544022003</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.2458915566478147</v>
       </c>
       <c r="C78">
@@ -2696,13 +2776,13 @@
         <v>0.32068602217968323</v>
       </c>
       <c r="H78">
-        <f ca="1">VLOOKUP(G78,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.31722963705823959</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.36240098974797175</v>
       </c>
       <c r="C79">
@@ -2721,13 +2801,13 @@
         <v>0.33227159518526728</v>
       </c>
       <c r="H79">
-        <f ca="1">VLOOKUP(G79,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.32832064101998426</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.87147050465467879</v>
       </c>
       <c r="C80">
@@ -2746,13 +2826,13 @@
         <v>0.33284561754969866</v>
       </c>
       <c r="H80">
-        <f ca="1">VLOOKUP(G80,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.32886917247420805</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.23718011017572782</v>
       </c>
       <c r="C81">
@@ -2771,13 +2851,13 @@
         <v>0.33360256140495403</v>
       </c>
       <c r="H81">
-        <f ca="1">VLOOKUP(G81,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.32959235687304278</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.28786506553522451</v>
       </c>
       <c r="C82">
@@ -2796,13 +2876,13 @@
         <v>0.35043383065927503</v>
       </c>
       <c r="H82">
-        <f ca="1">VLOOKUP(G82,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.34562918809953164</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.13500690479601085</v>
       </c>
       <c r="C83">
@@ -2821,13 +2901,13 @@
         <v>0.35301820822191921</v>
       </c>
       <c r="H83">
-        <f ca="1">VLOOKUP(G83,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.34808389993767541</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.47071881888696054</v>
       </c>
       <c r="C84">
@@ -2846,13 +2926,13 @@
         <v>0.36016834855198721</v>
       </c>
       <c r="H84">
-        <f ca="1">VLOOKUP(G84,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.35486412430581993</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.12274987953796856</v>
       </c>
       <c r="C85">
@@ -2871,13 +2951,13 @@
         <v>0.36240098974797175</v>
       </c>
       <c r="H85">
-        <f ca="1">VLOOKUP(G85,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.35697796361057893</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.95581828022028625</v>
       </c>
       <c r="C86">
@@ -2896,13 +2976,13 @@
         <v>0.36404804489053422</v>
       </c>
       <c r="H86">
-        <f ca="1">VLOOKUP(G86,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.35853639066496268</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.53116649632528667</v>
       </c>
       <c r="C87">
@@ -2921,13 +3001,13 @@
         <v>0.37356190579633497</v>
       </c>
       <c r="H87">
-        <f ca="1">VLOOKUP(G87,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.36752238603435822</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.83801505185631142</v>
       </c>
       <c r="C88">
@@ -2946,13 +3026,13 @@
         <v>0.37613373715978371</v>
       </c>
       <c r="H88">
-        <f ca="1">VLOOKUP(G88,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.36994693745258478</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>5.074436438629315E-2</v>
       </c>
       <c r="C89">
@@ -2971,13 +3051,13 @@
         <v>0.37661911437145701</v>
       </c>
       <c r="H89">
-        <f ca="1">VLOOKUP(G89,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.37040430818447945</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>4.0814367675169105E-2</v>
       </c>
       <c r="C90">
@@ -2996,13 +3076,13 @@
         <v>0.39145229848736818</v>
       </c>
       <c r="H90">
-        <f ca="1">VLOOKUP(G90,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.38435215082665064</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.65915462725000307</v>
       </c>
       <c r="C91">
@@ -3021,13 +3101,13 @@
         <v>0.39290796017087637</v>
       </c>
       <c r="H91">
-        <f ca="1">VLOOKUP(G91,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.38571811458433064</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.4969324041303701</v>
       </c>
       <c r="C92">
@@ -3046,13 +3126,13 @@
         <v>0.39817580068374037</v>
       </c>
       <c r="H92">
-        <f ca="1">VLOOKUP(G92,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.39065729342234146</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.12367011636589187</v>
       </c>
       <c r="C93">
@@ -3071,13 +3151,13 @@
         <v>0.39862711219381852</v>
       </c>
       <c r="H93">
-        <f ca="1">VLOOKUP(G93,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.39108016245478372</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.21195144677754441</v>
       </c>
       <c r="C94">
@@ -3096,13 +3176,13 @@
         <v>0.40825151308399987</v>
       </c>
       <c r="H94">
-        <f ca="1">VLOOKUP(G94,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.40008928126843413</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.97066156559272709</v>
       </c>
       <c r="C95">
@@ -3121,13 +3201,13 @@
         <v>0.41777394613903429</v>
       </c>
       <c r="H95">
-        <f ca="1">VLOOKUP(G95,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.40899026494523577</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.54442120069954791</v>
       </c>
       <c r="C96">
@@ -3146,13 +3226,13 @@
         <v>0.41913110104389739</v>
       </c>
       <c r="H96">
-        <f ca="1">VLOOKUP(G96,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.41025816851911939</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.63557681337531402</v>
       </c>
       <c r="C97">
@@ -3171,13 +3251,13 @@
         <v>0.42934979603996137</v>
       </c>
       <c r="H97">
-        <f ca="1">VLOOKUP(G97,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.41980026549653793</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.84604834000000917</v>
       </c>
       <c r="C98">
@@ -3196,13 +3276,13 @@
         <v>0.43415476418794674</v>
       </c>
       <c r="H98">
-        <f ca="1">VLOOKUP(G98,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.42428609571973341</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.98335274902263536</v>
       </c>
       <c r="C99">
@@ -3221,13 +3301,13 @@
         <v>0.4457537601902003</v>
       </c>
       <c r="H99">
-        <f ca="1">VLOOKUP(G99,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.43511796734543012</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.29120229052045066</v>
       </c>
       <c r="C100">
@@ -3246,13 +3326,13 @@
         <v>0.46103511851619938</v>
       </c>
       <c r="H100">
-        <f ca="1">VLOOKUP(G100,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.44941087642981736</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.39290796017087637</v>
       </c>
       <c r="C101">
@@ -3271,13 +3351,13 @@
         <v>0.47071881888696054</v>
       </c>
       <c r="H101">
-        <f ca="1">VLOOKUP(G101,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.45849163401404203</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.20732584521069475</v>
       </c>
       <c r="C102">
@@ -3296,13 +3376,13 @@
         <v>0.48754617572371206</v>
       </c>
       <c r="H102">
-        <f ca="1">VLOOKUP(G102,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.47433564354893609</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.95976967942117197</v>
       </c>
       <c r="C103">
@@ -3321,13 +3401,13 @@
         <v>0.49218259729089975</v>
       </c>
       <c r="H103">
-        <f ca="1">VLOOKUP(G103,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.47871878644192112</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.29376542857156063</v>
       </c>
       <c r="C104">
@@ -3346,13 +3426,13 @@
         <v>0.49491495918364981</v>
       </c>
       <c r="H104">
-        <f ca="1">VLOOKUP(G104,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.48130594107059887</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>3.2521870340801673E-2</v>
       </c>
       <c r="C105">
@@ -3371,13 +3451,13 @@
         <v>0.4969324041303701</v>
       </c>
       <c r="H105">
-        <f ca="1">VLOOKUP(G105,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.48321818551350854</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0.18384129893805279</v>
       </c>
       <c r="C106">
@@ -3396,13 +3476,13 @@
         <v>0.50176428454827404</v>
       </c>
       <c r="H106">
-        <f ca="1">VLOOKUP(G106,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0.48780533926566005</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107">
-        <f ca="1">RAND()</f>
+        <f t="shared" ref="A107:A138" ca="1" si="6">RAND()</f>
         <v>0.78368390074715666</v>
       </c>
       <c r="C107">
@@ -3421,13 +3501,13 @@
         <v>0.52623137132210263</v>
       </c>
       <c r="H107">
-        <f ca="1">VLOOKUP(G107,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ref="H107:H138" ca="1" si="7">VLOOKUP(G107,$C$11:$D$210,2,FALSE)</f>
         <v>0.51120712086453357</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>7.5311310574320056E-2</v>
       </c>
       <c r="C108">
@@ -3446,13 +3526,13 @@
         <v>0.53116649632528667</v>
       </c>
       <c r="H108">
-        <f ca="1">VLOOKUP(G108,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.51596571783122536</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.65165603119250037</v>
       </c>
       <c r="C109">
@@ -3471,13 +3551,13 @@
         <v>0.53620874545792085</v>
       </c>
       <c r="H109">
-        <f ca="1">VLOOKUP(G109,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.52084172822053176</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.94201043308537502</v>
       </c>
       <c r="C110">
@@ -3496,13 +3576,13 @@
         <v>0.5415391865705288</v>
       </c>
       <c r="H110">
-        <f ca="1">VLOOKUP(G110,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.52601220816260508</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.11942318801088558</v>
       </c>
       <c r="C111">
@@ -3521,13 +3601,13 @@
         <v>0.5416245349684724</v>
       </c>
       <c r="H111">
-        <f ca="1">VLOOKUP(G111,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.52609512840291461</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.98668215880595311</v>
       </c>
       <c r="C112">
@@ -3546,13 +3626,13 @@
         <v>0.54442120069954791</v>
       </c>
       <c r="H112">
-        <f ca="1">VLOOKUP(G112,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.52881456117750614</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.89033042792108408</v>
       </c>
       <c r="C113">
@@ -3571,13 +3651,13 @@
         <v>0.56326157593659643</v>
       </c>
       <c r="H113">
-        <f ca="1">VLOOKUP(G113,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.54725307372657939</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.68743417547964603</v>
       </c>
       <c r="C114">
@@ -3596,13 +3676,13 @@
         <v>0.56330163340138784</v>
       </c>
       <c r="H114">
-        <f ca="1">VLOOKUP(G114,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.54729249577187766</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.65729870798681056</v>
       </c>
       <c r="C115">
@@ -3621,13 +3701,13 @@
         <v>0.56671757809382073</v>
       </c>
       <c r="H115">
-        <f ca="1">VLOOKUP(G115,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.55065763107044963</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>2.7217525751247695E-2</v>
       </c>
       <c r="C116">
@@ -3646,13 +3726,13 @@
         <v>0.57117856170137415</v>
       </c>
       <c r="H116">
-        <f ca="1">VLOOKUP(G116,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.55506223411502065</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.89763996700680904</v>
       </c>
       <c r="C117">
@@ -3671,13 +3751,13 @@
         <v>0.57625729677356086</v>
       </c>
       <c r="H117">
-        <f ca="1">VLOOKUP(G117,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.56009062826567846</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.59334214411172115</v>
       </c>
       <c r="C118">
@@ -3696,13 +3776,13 @@
         <v>0.58677414175122655</v>
       </c>
       <c r="H118">
-        <f ca="1">VLOOKUP(G118,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.57054718897774948</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.88533356705178134</v>
       </c>
       <c r="C119">
@@ -3721,13 +3801,13 @@
         <v>0.58744770747225417</v>
       </c>
       <c r="H119">
-        <f ca="1">VLOOKUP(G119,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.57121884561708347</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.52623137132210263</v>
       </c>
       <c r="C120">
@@ -3746,13 +3826,13 @@
         <v>0.58907378796599141</v>
       </c>
       <c r="H120">
-        <f ca="1">VLOOKUP(G120,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.57284126939062485</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.37613373715978371</v>
       </c>
       <c r="C121">
@@ -3771,13 +3851,13 @@
         <v>0.59334214411172115</v>
       </c>
       <c r="H121">
-        <f ca="1">VLOOKUP(G121,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.57710646666364007</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.72973741777492462</v>
       </c>
       <c r="C122">
@@ -3796,13 +3876,13 @@
         <v>0.6021125217482759</v>
       </c>
       <c r="H122">
-        <f ca="1">VLOOKUP(G122,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.58589770082617021</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>8.1998452374188679E-2</v>
       </c>
       <c r="C123">
@@ -3821,13 +3901,13 @@
         <v>0.60295367400315036</v>
       </c>
       <c r="H123">
-        <f ca="1">VLOOKUP(G123,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.5867426678880453</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.4457537601902003</v>
       </c>
       <c r="C124">
@@ -3846,13 +3926,13 @@
         <v>0.6122368142980833</v>
       </c>
       <c r="H124">
-        <f ca="1">VLOOKUP(G124,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.59608800633867176</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.19206669044047031</v>
       </c>
       <c r="C125">
@@ -3871,13 +3951,13 @@
         <v>0.61311987827802683</v>
       </c>
       <c r="H125">
-        <f ca="1">VLOOKUP(G125,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.59697878652084901</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.39145229848736818</v>
       </c>
       <c r="C126">
@@ -3896,13 +3976,13 @@
         <v>0.61373471864774631</v>
       </c>
       <c r="H126">
-        <f ca="1">VLOOKUP(G126,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.59759917602818058</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.37661911437145701</v>
       </c>
       <c r="C127">
@@ -3921,13 +4001,13 @@
         <v>0.61649041736527788</v>
       </c>
       <c r="H127">
-        <f ca="1">VLOOKUP(G127,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.60038163390596022</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.58907378796599141</v>
       </c>
       <c r="C128">
@@ -3946,13 +4026,13 @@
         <v>0.61868751218167595</v>
       </c>
       <c r="H128">
-        <f ca="1">VLOOKUP(G128,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.60260191645747818</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.98199377601272875</v>
       </c>
       <c r="C129">
@@ -3971,13 +4051,13 @@
         <v>0.62058612926166434</v>
       </c>
       <c r="H129">
-        <f ca="1">VLOOKUP(G129,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.60452192981495645</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.80969128780519561</v>
       </c>
       <c r="C130">
@@ -3996,13 +4076,13 @@
         <v>0.62188519028793798</v>
       </c>
       <c r="H130">
-        <f ca="1">VLOOKUP(G130,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.60583648594532724</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.1753419963207854</v>
       </c>
       <c r="C131">
@@ -4021,13 +4101,13 @@
         <v>0.62392623342965237</v>
       </c>
       <c r="H131">
-        <f ca="1">VLOOKUP(G131,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.60790289430546096</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.6258207934425094</v>
       </c>
       <c r="C132">
@@ -4046,13 +4126,13 @@
         <v>0.62498956591875154</v>
       </c>
       <c r="H132">
-        <f ca="1">VLOOKUP(G132,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.60897987764952188</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.15262259680293022</v>
       </c>
       <c r="C133">
@@ -4071,13 +4151,13 @@
         <v>0.6258207934425094</v>
       </c>
       <c r="H133">
-        <f ca="1">VLOOKUP(G133,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.60982201901091981</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.82610133918910889</v>
       </c>
       <c r="C134">
@@ -4096,13 +4176,13 @@
         <v>0.62842158368510292</v>
       </c>
       <c r="H134">
-        <f ca="1">VLOOKUP(G134,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.61245828721935225</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.35043383065927503</v>
       </c>
       <c r="C135">
@@ -4121,13 +4201,13 @@
         <v>0.6289824602381856</v>
       </c>
       <c r="H135">
-        <f ca="1">VLOOKUP(G135,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.61302707097001941</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.69664327469498732</v>
       </c>
       <c r="C136">
@@ -4146,13 +4226,13 @@
         <v>0.63557681337531402</v>
       </c>
       <c r="H136">
-        <f ca="1">VLOOKUP(G136,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.61972066903337697</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.70126236854239865</v>
       </c>
       <c r="C137">
@@ -4171,13 +4251,13 @@
         <v>0.64104700133711212</v>
       </c>
       <c r="H137">
-        <f ca="1">VLOOKUP(G137,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.62528126340520296</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0.29668229901792387</v>
       </c>
       <c r="C138">
@@ -4196,13 +4276,13 @@
         <v>0.64473504063417375</v>
       </c>
       <c r="H138">
-        <f ca="1">VLOOKUP(G138,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0.62903335288013373</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139">
-        <f ca="1">RAND()</f>
+        <f t="shared" ref="A139:A170" ca="1" si="8">RAND()</f>
         <v>0.75018087921658505</v>
       </c>
       <c r="C139">
@@ -4221,13 +4301,13 @@
         <v>0.64812661935620586</v>
       </c>
       <c r="H139">
-        <f ca="1">VLOOKUP(G139,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ref="H139:H170" ca="1" si="9">VLOOKUP(G139,$C$11:$D$210,2,FALSE)</f>
         <v>0.63248582251463392</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.61868751218167595</v>
       </c>
       <c r="C140">
@@ -4246,13 +4326,13 @@
         <v>0.65165603119250037</v>
       </c>
       <c r="H140">
-        <f ca="1">VLOOKUP(G140,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.63608043377373691</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.50176428454827404</v>
       </c>
       <c r="C141">
@@ -4271,13 +4351,13 @@
         <v>0.65729870798681056</v>
       </c>
       <c r="H141">
-        <f ca="1">VLOOKUP(G141,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.6418299778212162</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.12204445810335407</v>
       </c>
       <c r="C142">
@@ -4296,13 +4376,13 @@
         <v>0.65915462725000307</v>
       </c>
       <c r="H142">
-        <f ca="1">VLOOKUP(G142,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.64372152253678483</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.58744770747225417</v>
       </c>
       <c r="C143">
@@ -4321,13 +4401,13 @@
         <v>0.6601836508485609</v>
       </c>
       <c r="H143">
-        <f ca="1">VLOOKUP(G143,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.64477037880936416</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.82643877356456308</v>
       </c>
       <c r="C144">
@@ -4346,13 +4426,13 @@
         <v>0.66416482932904097</v>
       </c>
       <c r="H144">
-        <f ca="1">VLOOKUP(G144,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.6488287930135791</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.91687018264790088</v>
       </c>
       <c r="C145">
@@ -4371,13 +4451,13 @@
         <v>0.66774505711271048</v>
       </c>
       <c r="H145">
-        <f ca="1">VLOOKUP(G145,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.65247864700989</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.6122368142980833</v>
       </c>
       <c r="C146">
@@ -4396,13 +4476,13 @@
         <v>0.67048525519173185</v>
       </c>
       <c r="H146">
-        <f ca="1">VLOOKUP(G146,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.65527186492214828</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.46103511851619938</v>
       </c>
       <c r="C147">
@@ -4421,13 +4501,13 @@
         <v>0.6748776782087198</v>
       </c>
       <c r="H147">
-        <f ca="1">VLOOKUP(G147,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.65974871075310548</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.56326157593659643</v>
       </c>
       <c r="C148">
@@ -4446,13 +4526,13 @@
         <v>0.68743417547964603</v>
       </c>
       <c r="H148">
-        <f ca="1">VLOOKUP(G148,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.67253552316653464</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.81182156457653665</v>
       </c>
       <c r="C149">
@@ -4471,13 +4551,13 @@
         <v>0.69325810791722031</v>
       </c>
       <c r="H149">
-        <f ca="1">VLOOKUP(G149,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.67845774349548416</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.36016834855198721</v>
       </c>
       <c r="C150">
@@ -4496,13 +4576,13 @@
         <v>0.69664327469498732</v>
       </c>
       <c r="H150">
-        <f ca="1">VLOOKUP(G150,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.68189707714147918</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.8272120972096304</v>
       </c>
       <c r="C151">
@@ -4521,13 +4601,13 @@
         <v>0.69739651627477239</v>
       </c>
       <c r="H151">
-        <f ca="1">VLOOKUP(G151,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.68266183153937876</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.26000782796753508</v>
       </c>
       <c r="C152">
@@ -4546,13 +4626,13 @@
         <v>0.70126236854239865</v>
       </c>
       <c r="H152">
-        <f ca="1">VLOOKUP(G152,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.68658434319718598</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.80552010318913791</v>
       </c>
       <c r="C153">
@@ -4571,13 +4651,13 @@
         <v>0.70536421020951268</v>
       </c>
       <c r="H153">
-        <f ca="1">VLOOKUP(G153,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.69074146522808233</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1.078728996835554E-2</v>
       </c>
       <c r="C154">
@@ -4596,13 +4676,13 @@
         <v>0.71132918410248991</v>
       </c>
       <c r="H154">
-        <f ca="1">VLOOKUP(G154,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.69677708400856309</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.96449719784768084</v>
       </c>
       <c r="C155">
@@ -4621,13 +4701,13 @@
         <v>0.71252772515564455</v>
       </c>
       <c r="H155">
-        <f ca="1">VLOOKUP(G155,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.69798818004123608</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.32017316355401948</v>
       </c>
       <c r="C156">
@@ -4646,13 +4726,13 @@
         <v>0.71942704459791362</v>
       </c>
       <c r="H156">
-        <f ca="1">VLOOKUP(G156,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.70494848883822947</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.39862711219381852</v>
       </c>
       <c r="C157">
@@ -4671,13 +4751,13 @@
         <v>0.71990193612817688</v>
       </c>
       <c r="H157">
-        <f ca="1">VLOOKUP(G157,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.70542683008912577</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.56671757809382073</v>
       </c>
       <c r="C158">
@@ -4696,13 +4776,13 @@
         <v>0.72973741777492462</v>
       </c>
       <c r="H158">
-        <f ca="1">VLOOKUP(G158,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.71531013182856418</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.27377111072492943</v>
       </c>
       <c r="C159">
@@ -4721,13 +4801,13 @@
         <v>0.73168113169364091</v>
       </c>
       <c r="H159">
-        <f ca="1">VLOOKUP(G159,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.71725753329284192</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.32043577670379675</v>
       </c>
       <c r="C160">
@@ -4746,13 +4826,13 @@
         <v>0.75018087921658505</v>
       </c>
       <c r="H160">
-        <f ca="1">VLOOKUP(G160,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.73568041132328776</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.89609171738393179</v>
       </c>
       <c r="C161">
@@ -4771,13 +4851,13 @@
         <v>0.76583932087094808</v>
       </c>
       <c r="H161">
-        <f ca="1">VLOOKUP(G161,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.75108969239643775</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.32045032100106585</v>
       </c>
       <c r="C162">
@@ -4796,13 +4876,13 @@
         <v>0.76713128008585307</v>
       </c>
       <c r="H162">
-        <f ca="1">VLOOKUP(G162,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.75235245652433047</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.23036853383573574</v>
       </c>
       <c r="C163">
@@ -4821,13 +4901,13 @@
         <v>0.78095119462370055</v>
       </c>
       <c r="H163">
-        <f ca="1">VLOOKUP(G163,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.76577002519357418</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>2.9796771519022824E-3</v>
       </c>
       <c r="C164">
@@ -4846,13 +4926,13 @@
         <v>0.78368390074715666</v>
       </c>
       <c r="H164">
-        <f ca="1">VLOOKUP(G164,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.7684024012672569</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.6748776782087198</v>
       </c>
       <c r="C165">
@@ -4871,13 +4951,13 @@
         <v>0.80063771429206632</v>
       </c>
       <c r="H165">
-        <f ca="1">VLOOKUP(G165,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.78456549905060802</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.71252772515564455</v>
       </c>
       <c r="C166">
@@ -4896,13 +4976,13 @@
         <v>0.80401721435042617</v>
       </c>
       <c r="H166">
-        <f ca="1">VLOOKUP(G166,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.78775056056013915</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.6021125217482759</v>
       </c>
       <c r="C167">
@@ -4921,13 +5001,13 @@
         <v>0.80552010318913791</v>
       </c>
       <c r="H167">
-        <f ca="1">VLOOKUP(G167,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.78916272580567737</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.86324843262165019</v>
       </c>
       <c r="C168">
@@ -4946,13 +5026,13 @@
         <v>0.80969128780519561</v>
       </c>
       <c r="H168">
-        <f ca="1">VLOOKUP(G168,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.79306831254341859</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.41913110104389739</v>
       </c>
       <c r="C169">
@@ -4971,13 +5051,13 @@
         <v>0.81182156457653665</v>
       </c>
       <c r="H169">
-        <f ca="1">VLOOKUP(G169,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.795055262960911</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0.17334968426002795</v>
       </c>
       <c r="C170">
@@ -4996,13 +5076,13 @@
         <v>0.81446791254319073</v>
       </c>
       <c r="H170">
-        <f ca="1">VLOOKUP(G170,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="9"/>
         <v>0.79751547388496757</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171">
-        <f ca="1">RAND()</f>
+        <f t="shared" ref="A171:A202" ca="1" si="10">RAND()</f>
         <v>0.5416245349684724</v>
       </c>
       <c r="C171">
@@ -5021,13 +5101,13 @@
         <v>0.82249681530953922</v>
       </c>
       <c r="H171">
-        <f ca="1">VLOOKUP(G171,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ref="H171:H202" ca="1" si="11">VLOOKUP(G171,$C$11:$D$210,2,FALSE)</f>
         <v>0.80492611193626573</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>1.7337165596859161E-2</v>
       </c>
       <c r="C172">
@@ -5046,13 +5126,13 @@
         <v>0.82610133918910889</v>
       </c>
       <c r="H172">
-        <f ca="1">VLOOKUP(G172,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.80822564158659427</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.66774505711271048</v>
       </c>
       <c r="C173">
@@ -5071,13 +5151,13 @@
         <v>0.82643877356456308</v>
       </c>
       <c r="H173">
-        <f ca="1">VLOOKUP(G173,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.80853363426642988</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.60295367400315036</v>
       </c>
       <c r="C174">
@@ -5096,13 +5176,13 @@
         <v>0.8272120972096304</v>
       </c>
       <c r="H174">
-        <f ca="1">VLOOKUP(G174,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.80923890302227386</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.6289824602381856</v>
       </c>
       <c r="C175">
@@ -5121,13 +5201,13 @@
         <v>0.83542490633498312</v>
       </c>
       <c r="H175">
-        <f ca="1">VLOOKUP(G175,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.81667834994475486</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>1.7122267577881489E-3</v>
       </c>
       <c r="C176">
@@ -5146,13 +5226,13 @@
         <v>0.83801505185631142</v>
       </c>
       <c r="H176">
-        <f ca="1">VLOOKUP(G176,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.8190045481430962</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.56330163340138784</v>
       </c>
       <c r="C177">
@@ -5171,13 +5251,13 @@
         <v>0.84604834000000917</v>
       </c>
       <c r="H177">
-        <f ca="1">VLOOKUP(G177,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.82615639186865897</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.53620874545792085</v>
       </c>
       <c r="C178">
@@ -5196,13 +5276,13 @@
         <v>0.8564682260373897</v>
       </c>
       <c r="H178">
-        <f ca="1">VLOOKUP(G178,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.83528318297024229</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.8564682260373897</v>
       </c>
       <c r="C179">
@@ -5221,13 +5301,13 @@
         <v>0.86324843262165019</v>
       </c>
       <c r="H179">
-        <f ca="1">VLOOKUP(G179,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.84112630054445248</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>6.6968298801553194E-2</v>
       </c>
       <c r="C180">
@@ -5246,13 +5326,13 @@
         <v>0.86500894223247471</v>
       </c>
       <c r="H180">
-        <f ca="1">VLOOKUP(G180,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.84263077998581626</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.39817580068374037</v>
       </c>
       <c r="C181">
@@ -5271,13 +5351,13 @@
         <v>0.87147050465467879</v>
       </c>
       <c r="H181">
-        <f ca="1">VLOOKUP(G181,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.84810564144862954</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.71132918410248991</v>
       </c>
       <c r="C182">
@@ -5296,13 +5376,13 @@
         <v>0.87600668101402845</v>
       </c>
       <c r="H182">
-        <f ca="1">VLOOKUP(G182,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.85190407673506385</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.64473504063417375</v>
       </c>
       <c r="C183">
@@ -5321,13 +5401,13 @@
         <v>0.88533356705178134</v>
       </c>
       <c r="H183">
-        <f ca="1">VLOOKUP(G183,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.85959254484233005</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.15296470412084306</v>
       </c>
       <c r="C184">
@@ -5346,13 +5426,13 @@
         <v>0.88889517457113931</v>
       </c>
       <c r="H184">
-        <f ca="1">VLOOKUP(G184,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.86248405521323024</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.49491495918364981</v>
       </c>
       <c r="C185">
@@ -5371,13 +5451,13 @@
         <v>0.88976342202478631</v>
       </c>
       <c r="H185">
-        <f ca="1">VLOOKUP(G185,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.86318528496452085</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.62058612926166434</v>
       </c>
       <c r="C186">
@@ -5396,13 +5476,13 @@
         <v>0.89033042792108408</v>
       </c>
       <c r="H186">
-        <f ca="1">VLOOKUP(G186,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.8636423010516282</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.27228545150351047</v>
       </c>
       <c r="C187">
@@ -5421,13 +5501,13 @@
         <v>0.89609171738393179</v>
       </c>
       <c r="H187">
-        <f ca="1">VLOOKUP(G187,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.86824974747333783</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.41777394613903429</v>
       </c>
       <c r="C188">
@@ -5446,13 +5526,13 @@
         <v>0.89763996700680904</v>
       </c>
       <c r="H188">
-        <f ca="1">VLOOKUP(G188,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.86947606052001947</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>8.991668778013151E-2</v>
       </c>
       <c r="C189">
@@ -5471,13 +5551,13 @@
         <v>0.90429427604463253</v>
       </c>
       <c r="H189">
-        <f ca="1">VLOOKUP(G189,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.87468927428028365</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.30165133066451744</v>
       </c>
       <c r="C190">
@@ -5496,13 +5576,13 @@
         <v>0.90509923036776352</v>
       </c>
       <c r="H190">
-        <f ca="1">VLOOKUP(G190,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.87531349191822894</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.27180867579582779</v>
       </c>
       <c r="C191">
@@ -5521,13 +5601,13 @@
         <v>0.90724442186076137</v>
       </c>
       <c r="H191">
-        <f ca="1">VLOOKUP(G191,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.8769706167034903</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.17888722108740762</v>
       </c>
       <c r="C192">
@@ -5546,13 +5626,13 @@
         <v>0.90949156806361353</v>
       </c>
       <c r="H192">
-        <f ca="1">VLOOKUP(G192,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.87869520236687804</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>6.4992667140739258E-2</v>
       </c>
       <c r="C193">
@@ -5571,13 +5651,13 @@
         <v>0.91687018264790088</v>
       </c>
       <c r="H193">
-        <f ca="1">VLOOKUP(G193,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.88427891693036165</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.62842158368510292</v>
       </c>
       <c r="C194">
@@ -5596,13 +5676,13 @@
         <v>0.917159763632167</v>
       </c>
       <c r="H194">
-        <f ca="1">VLOOKUP(G194,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.88449554708611033</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.35301820822191921</v>
       </c>
       <c r="C195">
@@ -5621,13 +5701,13 @@
         <v>0.9258348840460412</v>
       </c>
       <c r="H195">
-        <f ca="1">VLOOKUP(G195,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.89089546453786284</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.80063771429206632</v>
       </c>
       <c r="C196">
@@ -5646,13 +5726,13 @@
         <v>0.92766017343413176</v>
       </c>
       <c r="H196">
-        <f ca="1">VLOOKUP(G196,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.89221965850067952</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.18218204092391144</v>
       </c>
       <c r="C197">
@@ -5671,13 +5751,13 @@
         <v>0.94201043308537502</v>
       </c>
       <c r="H197">
-        <f ca="1">VLOOKUP(G197,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.90234823353828542</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.19281679903418802</v>
       </c>
       <c r="C198">
@@ -5696,13 +5776,13 @@
         <v>0.95581828022028625</v>
       </c>
       <c r="H198">
-        <f ca="1">VLOOKUP(G198,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.91160614327065437</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.76713128008585307</v>
       </c>
       <c r="C199">
@@ -5721,13 +5801,13 @@
         <v>0.95616580382950833</v>
       </c>
       <c r="H199">
-        <f ca="1">VLOOKUP(G199,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.91183278271743329</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.17510853168654139</v>
       </c>
       <c r="C200">
@@ -5746,13 +5826,13 @@
         <v>0.95685108731212942</v>
       </c>
       <c r="H200">
-        <f ca="1">VLOOKUP(G200,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.91227876714560341</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.73168113169364091</v>
       </c>
       <c r="C201">
@@ -5771,13 +5851,13 @@
         <v>0.95976967942117197</v>
       </c>
       <c r="H201">
-        <f ca="1">VLOOKUP(G201,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.91416437147880425</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0.12186110338312595</v>
       </c>
       <c r="C202">
@@ -5796,13 +5876,13 @@
         <v>0.96449719784768084</v>
       </c>
       <c r="H202">
-        <f ca="1">VLOOKUP(G202,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="11"/>
         <v>0.91717098102965877</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203">
-        <f ca="1">RAND()</f>
+        <f t="shared" ref="A203:A210" ca="1" si="12">RAND()</f>
         <v>0.57625729677356086</v>
       </c>
       <c r="C203">
@@ -5821,13 +5901,13 @@
         <v>0.96899087623978364</v>
       </c>
       <c r="H203">
-        <f ca="1">VLOOKUP(G203,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ref="H203:H210" ca="1" si="13">VLOOKUP(G203,$C$11:$D$210,2,FALSE)</f>
         <v>0.91997348002325063</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0.83542490633498312</v>
       </c>
       <c r="C204">
@@ -5846,13 +5926,13 @@
         <v>0.97066156559272709</v>
       </c>
       <c r="H204">
-        <f ca="1">VLOOKUP(G204,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0.92100148007664617</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0.62392623342965237</v>
       </c>
       <c r="C205">
@@ -5871,13 +5951,13 @@
         <v>0.98199377601272875</v>
       </c>
       <c r="H205">
-        <f ca="1">VLOOKUP(G205,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0.92777402608728654</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0.99936926495094447</v>
       </c>
       <c r="C206">
@@ -5896,13 +5976,13 @@
         <v>0.98335274902263536</v>
       </c>
       <c r="H206">
-        <f ca="1">VLOOKUP(G206,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0.92856244904397556</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0.917159763632167</v>
       </c>
       <c r="C207">
@@ -5921,13 +6001,13 @@
         <v>0.98668215880595311</v>
       </c>
       <c r="H207">
-        <f ca="1">VLOOKUP(G207,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0.93047243225787823</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0.17588953604697677</v>
       </c>
       <c r="C208">
@@ -5946,13 +6026,13 @@
         <v>0.99121748500782902</v>
       </c>
       <c r="H208">
-        <f ca="1">VLOOKUP(G208,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0.9330247960987138</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="12"/>
         <v>9.7837835960232544E-2</v>
       </c>
       <c r="C209">
@@ -5971,13 +6051,13 @@
         <v>0.9931097264999057</v>
       </c>
       <c r="H209">
-        <f ca="1">VLOOKUP(G209,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0.93407281432765465</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210">
-        <f ca="1">RAND()</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0.61373471864774631</v>
       </c>
       <c r="C210">
@@ -5996,7 +6076,7 @@
         <v>0.99936926495094447</v>
       </c>
       <c r="H210">
-        <f ca="1">VLOOKUP(G210,$C$11:$D$210,2,FALSE)</f>
+        <f t="shared" ca="1" si="13"/>
         <v>0.93746766618410737</v>
       </c>
     </row>
@@ -7671,7 +7751,7 @@
   <dimension ref="A1:H113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9323,8 +9403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8925CFF-550B-4B46-84E0-12321A16C437}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F10:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9455,7 +9535,7 @@
       </c>
       <c r="E11" t="str">
         <f ca="1"/>
-        <v/>
+        <v>Correlation</v>
       </c>
       <c r="F11">
         <f ca="1"/>

</xml_diff>